<commit_message>
Replacing CRID rloadest folders for TSS, pTHg, fTHg and CR8 TSS and pTHg; Replacing model results for TSS, pTHg, and fTHg; Adding Sigma Plot folder.
</commit_message>
<xml_diff>
--- a/2019_Combie_LoadsData_WY2018/Model Stats_rloadest/1_wy2018/1_fTHg_Model Results.xlsx
+++ b/2019_Combie_LoadsData_WY2018/Model Stats_rloadest/1_wy2018/1_fTHg_Model Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2019_Combie_LoadsData_WY2018\Model Stats_rloadest\1_wy2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE76105-1C37-423E-B79D-D10F75313215}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924A9252-C86E-48D5-844A-4BBCE4D7445E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24870" xr2:uid="{1DB9D86E-2E74-420B-9D3C-E44AD5ABCFD3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="9555" xr2:uid="{1DB9D86E-2E74-420B-9D3C-E44AD5ABCFD3}"/>
   </bookViews>
   <sheets>
     <sheet name="1_fTHg Model Results" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="440">
   <si>
     <t>closest to 1</t>
   </si>
@@ -856,6 +856,543 @@
   </si>
   <si>
     <t>fTHg wy 2018</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm1 &lt;- loadReg(fTHg ~model(1), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(1), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  The minimum spacing between daily loads is 4 days. The time between observations should be at least  7 days to avoid autocorrelation issues.</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 14</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2018.218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 5.6768</t>
+  </si>
+  <si>
+    <t>(Intercept)   -7.356     0.1965 -37.444       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.239     0.2056   6.026       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5307</t>
+  </si>
+  <si>
+    <t>R-squared: 75.16 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 19.5 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.7539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 1e-04</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.0326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Min 25% 50% 75% 90%  95%  Max</t>
+  </si>
+  <si>
+    <t>Est   0   0   0   0   0 0.01 0.01</t>
+  </si>
+  <si>
+    <t>Obs   0   0   0   0   0 0.02 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -26.76 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.08829</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm2 &lt;- loadReg(fTHg ~model(2), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(2), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Estimate Std. Error   z-score p-value</t>
+  </si>
+  <si>
+    <t>(Intercept) -7.351810     0.2995 -24.54981  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.238724     0.2147   5.76984  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.004874     0.2388  -0.02041  0.9816</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5789</t>
+  </si>
+  <si>
+    <t>G-squared: 19.5 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.755</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.0297</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -28.04 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.1011</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm3 &lt;- loadReg(fTHg ~model(3), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(3), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm3</t>
+  </si>
+  <si>
+    <t>(Intercept)  -7.3457     0.2017 -36.4270  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.2741     0.2168   5.8780  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME       0.5477     0.8092   0.6768  0.4498</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5558</t>
+  </si>
+  <si>
+    <t>R-squared: 76.16 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 20.07 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.7751</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.0353</t>
+  </si>
+  <si>
+    <t>lnQ     1.062</t>
+  </si>
+  <si>
+    <t>DECTIME 1.062</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -27.19 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.1082</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm4 &lt;- loadReg(fTHg ~model(4), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(4), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm4</t>
+  </si>
+  <si>
+    <t>(Intercept)  -7.3593     0.2015 -36.5145  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.2300     0.2133   5.7673  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.2971     0.2811   1.0569  0.2234</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.2541     0.2899  -0.8767  0.3086</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5299</t>
+  </si>
+  <si>
+    <t>R-squared: 79.34 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 22.07 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.8247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 4e-04</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.1354</t>
+  </si>
+  <si>
+    <t>lnQ         1.078</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 1.043</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 1.040</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -26.39 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.1617</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm5 &lt;- loadReg(fTHg ~model(5), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(5), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm5</t>
+  </si>
+  <si>
+    <t>(Intercept) -7.40087     0.3151 -23.4904  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.27924     0.2277   5.6169  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.06208     0.2633   0.2357  0.7806</t>
+  </si>
+  <si>
+    <t>DECTIME      0.62703     0.9108   0.6885  0.4207</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.608</t>
+  </si>
+  <si>
+    <t>R-squared: 76.29 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 20.15 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t>P-value: 0.0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.7813</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.0165</t>
+  </si>
+  <si>
+    <t>lnQ     1.072</t>
+  </si>
+  <si>
+    <t>lnQ2    1.158</t>
+  </si>
+  <si>
+    <t>DECTIME 1.229</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -27.61 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.1158</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm6 &lt;- loadReg(fTHg ~model(6), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(6), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm6</t>
+  </si>
+  <si>
+    <t>(Intercept)  -7.4269     0.3053 -24.3234  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.2344     0.2241   5.5083  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.0782     0.2546   0.3071  0.7024</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.2973     0.2947   1.0086  0.2208</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.2877     0.3230  -0.8906  0.2768</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5826</t>
+  </si>
+  <si>
+    <t>R-squared: 79.55 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 22.22 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.8376</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.114</t>
+  </si>
+  <si>
+    <t>lnQ         1.083</t>
+  </si>
+  <si>
+    <t>lnQ2        1.130</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 1.174</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -25.76 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7424</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.1612</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm7 &lt;- loadReg(fTHg ~model(7), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(7), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm7</t>
+  </si>
+  <si>
+    <t>(Intercept)  -7.3493     0.2060 -35.6741  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.1820     0.2262   5.2262  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -1.3823     1.7736  -0.7793  0.3390</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.4066     0.3194   1.2732  0.1278</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.6829     0.6246  -1.0933  0.1864</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5515</t>
+  </si>
+  <si>
+    <t>R-squared: 80.64 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 22.99 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t>P-value: 0.0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.851</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0011</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.2354</t>
+  </si>
+  <si>
+    <t>lnQ         1.165</t>
+  </si>
+  <si>
+    <t>DECTIME     5.140</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 1.293</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 4.638</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -26.22 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.2001</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm8 &lt;- loadReg(fTHg ~model(8), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(8), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm8</t>
+  </si>
+  <si>
+    <t>(Intercept) -7.38881     0.3193 -23.1409  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.18651     0.2410   4.9241  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.04512     0.2666   0.1693  0.8230</t>
+  </si>
+  <si>
+    <t>DECTIME     -1.32450     1.9086  -0.6940  0.3657</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  0.40218     0.3392   1.1858  0.1322</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.68435     0.6614  -1.0347  0.1848</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.6182</t>
+  </si>
+  <si>
+    <t>R-squared: 80.71 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 23.04 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t>P-value: 0.0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.8525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0012</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.2142</t>
+  </si>
+  <si>
+    <t>lnQ         1.180</t>
+  </si>
+  <si>
+    <t>lnQ2        1.167</t>
+  </si>
+  <si>
+    <t>DECTIME     5.310</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 1.301</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -26.99 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.2134</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm9 &lt;- loadReg(fTHg ~model(9), data = fTHg_CR1D, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "Combie-In")</t>
+  </si>
+  <si>
+    <t>In loadReg(fTHg ~ model(9), data = fTHg_CR1D, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; fTHg_CR1Dm9</t>
+  </si>
+  <si>
+    <t>(Intercept) -9.42204     1.5303 -6.1568  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.16219     0.2300  5.0539  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.07264     0.2681 -0.2709  0.7024</t>
+  </si>
+  <si>
+    <t>DECTIME     -3.03489     2.2112 -1.3725  0.0678</t>
+  </si>
+  <si>
+    <t>DECTIME2    27.56633    20.3353  1.3556  0.0708</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  2.84429     1.8302  1.5541  0.0416</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.70369     0.6294 -1.1180  0.1294</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5596</t>
+  </si>
+  <si>
+    <t>R-squared: 84.72 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 26.3 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.8669</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.3407</t>
+  </si>
+  <si>
+    <t>lnQ          1.187</t>
+  </si>
+  <si>
+    <t>lnQ2         1.304</t>
+  </si>
+  <si>
+    <t>DECTIME      7.873</t>
+  </si>
+  <si>
+    <t>DECTIME2    39.079</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 41.857</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  4.641</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -25.52 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.7448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.2977</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 14; Period of record: 2017-11-02 to 2018-08-27</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1187,7 +1724,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1211,10 +1754,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1928,7 +2468,8 @@
   <dimension ref="A1:AH83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1936,7 +2477,9 @@
     <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" style="2" customWidth="1"/>
     <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="14" width="10.7109375" style="2" customWidth="1"/>
+    <col min="8" max="11" width="10.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="10.7109375" style="2" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -1944,24 +2487,24 @@
       <c r="A1" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35" t="s">
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="35"/>
+      <c r="M1" s="45"/>
       <c r="N1" s="23"/>
       <c r="O1" s="23"/>
     </row>
@@ -2087,18 +2630,18 @@
     </row>
     <row r="5" spans="1:34" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
       <c r="Y6" s="5" t="s">
         <v>2</v>
       </c>
@@ -2113,22 +2656,22 @@
       <c r="AH6" s="5"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="41" t="s">
         <v>243</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="42" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="42"/>
+      <c r="M7" s="44"/>
       <c r="Y7" s="5" t="s">
         <v>4</v>
       </c>
@@ -2250,16 +2793,16 @@
       <c r="C10" s="28">
         <v>8.0100000000000005E-2</v>
       </c>
-      <c r="D10" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="43" t="s">
+      <c r="D10" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="36" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="16" t="s">
@@ -2280,7 +2823,7 @@
       <c r="M10" s="16">
         <v>0.98650000000000004</v>
       </c>
-      <c r="N10" s="44" t="s">
+      <c r="N10" s="37" t="s">
         <v>244</v>
       </c>
       <c r="O10" s="14" t="s">
@@ -2654,18 +3197,18 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="40"/>
       <c r="L19" s="23"/>
       <c r="M19" s="23"/>
       <c r="N19" s="23"/>
@@ -2682,20 +3225,22 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="23"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="42" t="s">
+      <c r="B20" s="41" t="s">
+        <v>439</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="M20" s="42"/>
+      <c r="M20" s="44"/>
       <c r="N20" s="23"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
@@ -2756,48 +3301,69 @@
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A22" s="23">
+      <c r="A22" s="16">
         <v>1</v>
       </c>
       <c r="B22" s="16">
         <v>0</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="9" t="s">
+      <c r="C22" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="36" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="10"/>
-      <c r="Q22" s="10"/>
+      <c r="I22" s="16">
+        <v>75.16</v>
+      </c>
+      <c r="J22" s="28">
+        <v>1E-4</v>
+      </c>
+      <c r="K22" s="16">
+        <v>3.2599999999999997E-2</v>
+      </c>
+      <c r="L22" s="16">
+        <v>-26.76</v>
+      </c>
+      <c r="M22" s="16">
+        <v>8.8289999999999993E-2</v>
+      </c>
+      <c r="N22" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q22" s="14" t="s">
+        <v>262</v>
+      </c>
       <c r="Z22" s="10"/>
+      <c r="AA22" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="23">
         <v>2</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="12">
         <v>0</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="11">
+        <v>0.98160000000000003</v>
+      </c>
       <c r="D23" s="9" t="s">
         <v>19</v>
       </c>
@@ -2810,30 +3376,49 @@
       <c r="G23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
+      <c r="I23" s="35">
+        <v>75.16</v>
+      </c>
+      <c r="J23" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="K23" s="35">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="L23" s="35">
+        <v>-28.04</v>
+      </c>
+      <c r="M23" s="35">
+        <v>0.1011</v>
+      </c>
       <c r="N23" s="23"/>
-      <c r="O23" s="10"/>
-      <c r="Q23" s="10"/>
+      <c r="O23" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>284</v>
+      </c>
       <c r="Z23" s="10"/>
+      <c r="AA23" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>3</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="12">
         <v>0</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="13"/>
+      <c r="D24" s="13">
+        <v>0.44979999999999998</v>
+      </c>
       <c r="E24" s="9" t="s">
         <v>19</v>
       </c>
@@ -2843,24 +3428,41 @@
       <c r="G24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
+      <c r="I24" s="12">
+        <v>76.16</v>
+      </c>
+      <c r="J24" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="K24" s="12">
+        <v>-3.5299999999999998E-2</v>
+      </c>
+      <c r="L24" s="12">
+        <v>-27.19</v>
+      </c>
+      <c r="M24" s="12">
+        <v>0.1082</v>
+      </c>
       <c r="N24" s="12"/>
-      <c r="O24" s="10"/>
-      <c r="Q24" s="10"/>
+      <c r="O24" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q24" s="14" t="s">
+        <v>298</v>
+      </c>
       <c r="Z24" s="10"/>
+      <c r="AA24" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="23">
         <v>4</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="12">
         <v>0</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -2872,30 +3474,55 @@
       <c r="E25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="16" t="s">
+      <c r="F25" s="12">
+        <v>0.22339999999999999</v>
+      </c>
+      <c r="G25" s="35">
+        <v>0.30859999999999999</v>
+      </c>
+      <c r="H25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
+      <c r="I25" s="35">
+        <v>79.34</v>
+      </c>
+      <c r="J25" s="11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="K25" s="35">
+        <v>-0.13539999999999999</v>
+      </c>
+      <c r="L25" s="35">
+        <v>-26.39</v>
+      </c>
+      <c r="M25" s="35">
+        <v>0.16170000000000001</v>
+      </c>
       <c r="N25" s="23"/>
-      <c r="O25" s="10"/>
-      <c r="Q25" s="10"/>
+      <c r="O25" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q25" s="14" t="s">
+        <v>314</v>
+      </c>
       <c r="Z25" s="10"/>
+      <c r="AA25" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="23">
         <v>5</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="12">
         <v>0</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
+      <c r="C26" s="35">
+        <v>0.78059999999999996</v>
+      </c>
+      <c r="D26" s="35">
+        <v>0.42070000000000002</v>
+      </c>
       <c r="E26" s="9" t="s">
         <v>19</v>
       </c>
@@ -2905,128 +3532,243 @@
       <c r="G26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
+      <c r="H26" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I26" s="35">
+        <v>76.290000000000006</v>
+      </c>
+      <c r="J26" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="K26" s="35">
+        <v>-1.6500000000000001E-2</v>
+      </c>
+      <c r="L26" s="35">
+        <v>-27.61</v>
+      </c>
+      <c r="M26" s="35">
+        <v>0.1158</v>
+      </c>
       <c r="N26" s="23"/>
-      <c r="O26" s="10"/>
-      <c r="Q26" s="10"/>
+      <c r="O26" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q26" s="14" t="s">
+        <v>333</v>
+      </c>
       <c r="Z26" s="10"/>
+      <c r="AA26" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="23">
         <v>6</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="12">
         <v>0</v>
       </c>
-      <c r="C27" s="34"/>
+      <c r="C27" s="35">
+        <v>0.70240000000000002</v>
+      </c>
       <c r="D27" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
+      <c r="F27" s="12">
+        <v>0.2208</v>
+      </c>
+      <c r="G27" s="35">
+        <v>0.27679999999999999</v>
+      </c>
+      <c r="H27" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I27" s="35">
+        <v>79.55</v>
+      </c>
+      <c r="J27" s="11">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="K27" s="35">
+        <v>-0.114</v>
+      </c>
+      <c r="L27" s="35">
+        <v>-25.76</v>
+      </c>
+      <c r="M27" s="35">
+        <v>0.16120000000000001</v>
+      </c>
       <c r="N27" s="23"/>
-      <c r="O27" s="10"/>
-      <c r="Q27" s="10"/>
+      <c r="O27" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q27" s="14" t="s">
+        <v>352</v>
+      </c>
       <c r="Z27" s="10"/>
+      <c r="AA27" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="23">
         <v>7</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <v>0</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="12"/>
+      <c r="D28" s="12">
+        <v>0.33900000000000002</v>
+      </c>
       <c r="E28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
+      <c r="F28" s="12">
+        <v>0.1278</v>
+      </c>
+      <c r="G28" s="35">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="I28" s="35">
+        <v>80.64</v>
+      </c>
+      <c r="J28" s="35">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="K28" s="35">
+        <v>-0.2354</v>
+      </c>
+      <c r="L28" s="35">
+        <v>-26.22</v>
+      </c>
+      <c r="M28" s="35">
+        <v>0.2001</v>
+      </c>
       <c r="N28" s="23"/>
-      <c r="O28" s="10"/>
-      <c r="Q28" s="10"/>
+      <c r="O28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q28" s="14" t="s">
+        <v>371</v>
+      </c>
       <c r="Z28" s="10"/>
+      <c r="AA28" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="23">
         <v>8</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="12">
         <v>0</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="12"/>
+      <c r="C29" s="35">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0.36570000000000003</v>
+      </c>
       <c r="E29" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
+      <c r="F29" s="12">
+        <v>0.13220000000000001</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0.18479999999999999</v>
+      </c>
+      <c r="H29" s="12">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="I29" s="35">
+        <v>80.709999999999994</v>
+      </c>
+      <c r="J29" s="35">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K29" s="35">
+        <v>-0.2142</v>
+      </c>
+      <c r="L29" s="35">
+        <v>-26.99</v>
+      </c>
+      <c r="M29" s="35">
+        <v>0.21340000000000001</v>
+      </c>
       <c r="N29" s="23"/>
-      <c r="O29" s="10"/>
-      <c r="Q29" s="10"/>
+      <c r="O29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q29" s="14" t="s">
+        <v>393</v>
+      </c>
       <c r="Z29" s="10"/>
+      <c r="AA29" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" s="23">
         <v>9</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <v>0</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
+      <c r="C30" s="12">
+        <v>0.70240000000000002</v>
+      </c>
+      <c r="D30" s="12">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="E30" s="12">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="F30" s="12">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0.12939999999999999</v>
+      </c>
+      <c r="H30" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I30" s="35">
+        <v>84.72</v>
+      </c>
+      <c r="J30" s="12">
+        <v>2E-3</v>
+      </c>
+      <c r="K30" s="35">
+        <v>-0.3407</v>
+      </c>
+      <c r="L30" s="35">
+        <v>-25.52</v>
+      </c>
+      <c r="M30" s="35">
+        <v>0.29770000000000002</v>
+      </c>
       <c r="N30" s="23"/>
-      <c r="O30" s="10"/>
-      <c r="Q30" s="10"/>
+      <c r="O30" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q30" s="14" t="s">
+        <v>416</v>
+      </c>
       <c r="Z30" s="10"/>
+      <c r="AA30" s="15" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="23"/>
@@ -3046,38 +3788,38 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" s="23"/>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="38"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="40"/>
       <c r="L32" s="23"/>
       <c r="M32" s="23"/>
       <c r="N32" s="23"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="23"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="42" t="s">
+      <c r="B33" s="41"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="M33" s="42"/>
+      <c r="M33" s="44"/>
       <c r="N33" s="23"/>
     </row>
     <row r="34" spans="1:28" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3420,36 +4162,36 @@
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="23"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="38"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="40"/>
       <c r="L45" s="23"/>
       <c r="M45" s="23"/>
       <c r="N45" s="23"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="23"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="42" t="s">
+      <c r="B46" s="41"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="M46" s="42"/>
+      <c r="M46" s="44"/>
       <c r="N46" s="23"/>
     </row>
     <row r="47" spans="1:28" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3790,36 +4532,36 @@
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="23"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="38"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="40"/>
       <c r="L58" s="23"/>
       <c r="M58" s="23"/>
       <c r="N58" s="23"/>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="23"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="41"/>
-      <c r="L59" s="42" t="s">
+      <c r="B59" s="41"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
+      <c r="H59" s="42"/>
+      <c r="I59" s="42"/>
+      <c r="J59" s="42"/>
+      <c r="K59" s="43"/>
+      <c r="L59" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="M59" s="42"/>
+      <c r="M59" s="44"/>
       <c r="N59" s="23"/>
     </row>
     <row r="60" spans="1:28" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4158,36 +4900,36 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="23"/>
-      <c r="B72" s="36"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="37"/>
-      <c r="I72" s="37"/>
-      <c r="J72" s="37"/>
-      <c r="K72" s="38"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="39"/>
+      <c r="I72" s="39"/>
+      <c r="J72" s="39"/>
+      <c r="K72" s="40"/>
       <c r="L72" s="23"/>
       <c r="M72" s="23"/>
       <c r="N72" s="23"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="23"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40"/>
-      <c r="E73" s="40"/>
-      <c r="F73" s="40"/>
-      <c r="G73" s="40"/>
-      <c r="H73" s="40"/>
-      <c r="I73" s="40"/>
-      <c r="J73" s="40"/>
-      <c r="K73" s="41"/>
-      <c r="L73" s="42" t="s">
+      <c r="B73" s="41"/>
+      <c r="C73" s="42"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
+      <c r="F73" s="42"/>
+      <c r="G73" s="42"/>
+      <c r="H73" s="42"/>
+      <c r="I73" s="42"/>
+      <c r="J73" s="42"/>
+      <c r="K73" s="43"/>
+      <c r="L73" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="M73" s="42"/>
+      <c r="M73" s="44"/>
       <c r="N73" s="23"/>
     </row>
     <row r="74" spans="1:15" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4494,6 +5236,19 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="B20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="B45:K45"/>
     <mergeCell ref="B72:K72"/>
     <mergeCell ref="B73:K73"/>
     <mergeCell ref="L73:M73"/>
@@ -4502,19 +5257,6 @@
     <mergeCell ref="B58:K58"/>
     <mergeCell ref="B59:K59"/>
     <mergeCell ref="L59:M59"/>
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="B33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B19:K19"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B6:K6"/>
   </mergeCells>
   <conditionalFormatting sqref="L103:L1048576">
     <cfRule type="cellIs" dxfId="38" priority="71" operator="between">
@@ -7148,13 +7890,2459 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782ED82D-3F7D-4A0C-8395-394E001D5349}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A524"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="25" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="24"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="24"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="24"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="24"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="26" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="26" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="26" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="24"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="26" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="26" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="26" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="24"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="24"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="24"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="26" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="26" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="26" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="24"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="25" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="25" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="24"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="24"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="24"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="24"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="24"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="26" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="26" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="24"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="26" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="26" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="26" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="26" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="24"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="26" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="24"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="24"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="26" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="26" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="26" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="24"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="25" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="14" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="25" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="24"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="24"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="24"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="24"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="24"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="26" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="26" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="26" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="24"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="26" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="26" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="26" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="24"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="26" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="24"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="24"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="26" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="24"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="25" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="14" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="25" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="24"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="24"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="24"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="24"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="24"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="26" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="24"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="26" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="26" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="26" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="26" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="26" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="26" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="24"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="26" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="26" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="26" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="24"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="24"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="26" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="26" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="26" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="24"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="25" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="25" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="24"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="24"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="24"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="24"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="24"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="26" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="26" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="26" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="26" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="24"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="26" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="26" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="26" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="26" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="26" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="26" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="24"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="26" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="26" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="26" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="24"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="24"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="26" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="26" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="26" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="24"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="25" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="25" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="24"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="24"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="24"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="24"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="24"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="26" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="26" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="26" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="26" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="26" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="24"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="26" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="26" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="26" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="26" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="26" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="26" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="26" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="24"/>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="26" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="26" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="26" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="26" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="24"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="24"/>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="26" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="26" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="26" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="24"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="25" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="14" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="25" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="24"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="24"/>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="24"/>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="24"/>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="24"/>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="26" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="26" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="26" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="26" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="26" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="26" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="24"/>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="26" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="26" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="26" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="26" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="26" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="26" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="24"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="26" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="26" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="26" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="26" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="26" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="24"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="24"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="26" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="26" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="26" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="24"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="25" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="14" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="25" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="24"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="24"/>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="24"/>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="24"/>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="26" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="24"/>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="26" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="26" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="26" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="26" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="26" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="26" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="26" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="24"/>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="26" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="26" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="26" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="26" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="26" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="26" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="24"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="26" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="26" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="26" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="26" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="26" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="26" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="24"/>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="24"/>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="26" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="26" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="27" t="s">
+        <v>438</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>